<commit_message>
Work on Input Capture Module
Solution has been founded for frequency up to 50KHz.
From 50KHz, input capture buffer runs in overflow. This issus must be fixed.
</commit_message>
<xml_diff>
--- a/Measures/AccuracyInputCapture.xlsx
+++ b/Measures/AccuracyInputCapture.xlsx
@@ -112,8 +112,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A3:C12" totalsRowShown="0">
-  <autoFilter ref="A3:C12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A3:C13" totalsRowShown="0">
+  <autoFilter ref="A3:C13"/>
   <sortState ref="A10:C18">
     <sortCondition ref="A9:A18"/>
   </sortState>
@@ -394,7 +394,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -430,7 +430,7 @@
         <v>0.10000089500000001</v>
       </c>
       <c r="C4" s="1">
-        <f>B4/(A4/100)-100</f>
+        <f t="shared" ref="C4:C12" si="0">B4/(A4/100)-100</f>
         <v>8.9499999999986812E-4</v>
       </c>
     </row>
@@ -442,7 +442,7 @@
         <v>1.0000110129999999</v>
       </c>
       <c r="C5" s="1">
-        <f>B5/(A5/100)-100</f>
+        <f t="shared" si="0"/>
         <v>1.1012999999877593E-3</v>
       </c>
     </row>
@@ -454,7 +454,7 @@
         <v>10.000318760000001</v>
       </c>
       <c r="C6" s="1">
-        <f>B6/(A6/100)-100</f>
+        <f t="shared" si="0"/>
         <v>3.1876000000039539E-3</v>
       </c>
     </row>
@@ -466,7 +466,7 @@
         <v>100.0258817</v>
       </c>
       <c r="C7" s="1">
-        <f>B7/(A7/100)-100</f>
+        <f t="shared" si="0"/>
         <v>2.5881699999999341E-2</v>
       </c>
     </row>
@@ -478,7 +478,7 @@
         <v>250.15243659999999</v>
       </c>
       <c r="C8" s="1">
-        <f>B8/(A8/100)-100</f>
+        <f t="shared" si="0"/>
         <v>6.0974639999997748E-2</v>
       </c>
     </row>
@@ -490,7 +490,7 @@
         <v>500.60385339999999</v>
       </c>
       <c r="C9" s="1">
-        <f>B9/(A9/100)-100</f>
+        <f t="shared" si="0"/>
         <v>0.12077067999999258</v>
       </c>
     </row>
@@ -502,7 +502,7 @@
         <v>1002.167187</v>
       </c>
       <c r="C10" s="1">
-        <f>B10/(A10/100)-100</f>
+        <f t="shared" si="0"/>
         <v>0.21671870000000126</v>
       </c>
     </row>
@@ -514,7 +514,7 @@
         <v>10234.105159999999</v>
       </c>
       <c r="C11" s="1">
-        <f>B11/(A11/100)-100</f>
+        <f t="shared" si="0"/>
         <v>2.3410515999999859</v>
       </c>
     </row>
@@ -526,8 +526,20 @@
         <v>220385.67</v>
       </c>
       <c r="C12" s="1">
-        <f>B12/(A12/100)-100</f>
+        <f t="shared" si="0"/>
         <v>120.38567</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>150000</v>
+      </c>
+      <c r="B13" s="1">
+        <v>150093.81</v>
+      </c>
+      <c r="C13" s="1">
+        <f>B13/(A13/100)-100</f>
+        <v>6.2539999999998486E-2</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>